<commit_message>
Correções no R Shiny App
</commit_message>
<xml_diff>
--- a/relatorios/base de dados/CONDOMINIO UP JARDIM PRUDENCIA ECN 2024_07_03 11_00_17.xlsx
+++ b/relatorios/base de dados/CONDOMINIO UP JARDIM PRUDENCIA ECN 2024_07_03 11_00_17.xlsx
@@ -3996,13 +3996,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09E4213A-557D-4DAD-8EAC-200A46C505E3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AE10D5D-D531-4CD2-9BBB-2BA97550CDC5}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F926ACD-D3D1-477D-9F8D-0A3E38680705}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D145F24-1C70-419C-94D7-65D0871A1D6D}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE1E0C68-7F2B-4954-9B4E-649AAC96C6F3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01B26237-619D-4BFE-85B9-7E90D84C0B22}"/>
 </file>
</xml_diff>

<commit_message>
Excluindo ECNs em xlsx
Anteriormente, a função "extrair_dados_arquivo_ecn()" criava os ECNs em xlsx em "Ampla_Github". Isso foi alterado para que os arquivos sejam criados nas respectivas pastas de onde vieram.
</commit_message>
<xml_diff>
--- a/relatorios/base de dados/CONDOMINIO UP JARDIM PRUDENCIA ECN 2024_07_03 11_00_17.xlsx
+++ b/relatorios/base de dados/CONDOMINIO UP JARDIM PRUDENCIA ECN 2024_07_03 11_00_17.xlsx
@@ -3996,13 +3996,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AE10D5D-D531-4CD2-9BBB-2BA97550CDC5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A62FFB78-ECCD-4F19-8CE9-9164C469D674}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D145F24-1C70-419C-94D7-65D0871A1D6D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26C7EF76-72F1-4767-BB66-AA3E3A4E3FC8}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01B26237-619D-4BFE-85B9-7E90D84C0B22}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A128701-CDC1-4AEB-AB68-28EDC0F6A57F}"/>
 </file>
</xml_diff>